<commit_message>
sube ultimos cambios e informe final
</commit_message>
<xml_diff>
--- a/python/Buck/resources/duty.xlsx
+++ b/python/Buck/resources/duty.xlsx
@@ -49,7 +49,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -61,10 +61,6 @@
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -187,8 +183,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -410,7 +410,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>